<commit_message>
Not matching elements structure rearranged
</commit_message>
<xml_diff>
--- a/media/testSet2/mergedFile.xlsx
+++ b/media/testSet2/mergedFile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3984" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="1124">
   <si>
     <t>Particulars</t>
   </si>
@@ -40155,13 +40155,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -40186,32 +40186,8 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -40239,32 +40215,8 @@
       <c r="I2">
         <v>3781.98</v>
       </c>
-      <c r="J2">
-        <v>7</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -40292,32 +40244,8 @@
       <c r="I3">
         <v>160.52</v>
       </c>
-      <c r="J3">
-        <v>16</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -40345,32 +40273,8 @@
       <c r="I4">
         <v>146.58</v>
       </c>
-      <c r="J4">
-        <v>17</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -40398,32 +40302,8 @@
       <c r="I5">
         <v>546.16</v>
       </c>
-      <c r="J5">
-        <v>39</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -40451,32 +40331,8 @@
       <c r="I6">
         <v>7033.96</v>
       </c>
-      <c r="J6">
-        <v>1553</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -40504,32 +40360,8 @@
       <c r="I7">
         <v>81</v>
       </c>
-      <c r="J7">
-        <v>63</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -40557,32 +40389,8 @@
       <c r="I8">
         <v>102.6</v>
       </c>
-      <c r="J8">
-        <v>102</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -40610,32 +40418,8 @@
       <c r="I9">
         <v>3051.9</v>
       </c>
-      <c r="J9">
-        <v>12</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -40663,32 +40447,8 @@
       <c r="I10">
         <v>198.58</v>
       </c>
-      <c r="J10">
-        <v>61</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -40716,32 +40476,8 @@
       <c r="I11">
         <v>2451.6</v>
       </c>
-      <c r="J11">
-        <v>671</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -40769,32 +40505,8 @@
       <c r="I12">
         <v>741.8</v>
       </c>
-      <c r="J12">
-        <v>1626</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -40822,32 +40534,8 @@
       <c r="I13">
         <v>3585.24</v>
       </c>
-      <c r="J13">
-        <v>15</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -40875,32 +40563,8 @@
       <c r="I14">
         <v>874.8</v>
       </c>
-      <c r="J14">
-        <v>34</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -40928,32 +40592,8 @@
       <c r="I15">
         <v>1360.98</v>
       </c>
-      <c r="J15">
-        <v>50</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -40981,32 +40621,8 @@
       <c r="I16">
         <v>85.22</v>
       </c>
-      <c r="J16">
-        <v>88</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -41034,32 +40650,8 @@
       <c r="I17">
         <v>636.8200000000001</v>
       </c>
-      <c r="J17">
-        <v>89</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -41087,32 +40679,8 @@
       <c r="I18">
         <v>744.48</v>
       </c>
-      <c r="J18">
-        <v>1690</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -41140,32 +40708,8 @@
       <c r="I19">
         <v>91.8</v>
       </c>
-      <c r="J19">
-        <v>10143</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -41193,32 +40737,8 @@
       <c r="I20">
         <v>494.02</v>
       </c>
-      <c r="J20">
-        <v>12</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -41246,32 +40766,8 @@
       <c r="I21">
         <v>197.18</v>
       </c>
-      <c r="J21">
-        <v>113</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -41299,32 +40795,8 @@
       <c r="I22">
         <v>521.34</v>
       </c>
-      <c r="J22">
-        <v>114</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -41351,30 +40823,6 @@
       </c>
       <c r="I23">
         <v>1732963.11</v>
-      </c>
-      <c r="J23" t="s">
-        <v>609</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -41384,83 +40832,59 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>172</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
+        <v>681</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1104</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>22054.2</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>18690</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>3364.2</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -41468,52 +40892,28 @@
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2">
-        <v>411</v>
-      </c>
-      <c r="K2" t="s">
-        <v>681</v>
-      </c>
-      <c r="L2" t="s">
-        <v>1104</v>
-      </c>
-      <c r="M2">
-        <v>22054.2</v>
-      </c>
-      <c r="N2">
-        <v>18690</v>
-      </c>
-      <c r="O2">
-        <v>3364.2</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>0</v>
+      <c r="B3" t="s">
+        <v>173</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+        <v>682</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1105</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>2501</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>2501</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>125.05</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -41521,52 +40921,28 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="J3">
-        <v>19000210</v>
-      </c>
-      <c r="K3" t="s">
-        <v>682</v>
-      </c>
-      <c r="L3" t="s">
-        <v>1105</v>
-      </c>
-      <c r="M3">
-        <v>2501</v>
-      </c>
-      <c r="N3">
-        <v>2501</v>
-      </c>
-      <c r="O3">
-        <v>125.05</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>173</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
+        <v>682</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1106</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1088</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1088</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>54.4</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -41574,370 +40950,202 @@
       <c r="I4">
         <v>0</v>
       </c>
-      <c r="J4">
-        <v>19000542</v>
-      </c>
-      <c r="K4" t="s">
-        <v>682</v>
-      </c>
-      <c r="L4" t="s">
-        <v>1106</v>
-      </c>
-      <c r="M4">
-        <v>1088</v>
-      </c>
-      <c r="N4">
-        <v>1088</v>
-      </c>
-      <c r="O4">
-        <v>54.4</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>0</v>
+      <c r="B5" t="s">
+        <v>102</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
+        <v>617</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1107</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>24793</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>21011.08</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1891</v>
       </c>
       <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5" t="s">
-        <v>617</v>
-      </c>
-      <c r="L5" t="s">
-        <v>1107</v>
-      </c>
-      <c r="M5">
-        <v>24793</v>
-      </c>
-      <c r="N5">
-        <v>21011.08</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
         <v>1891</v>
       </c>
-      <c r="Q5">
-        <v>1891</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>0</v>
+      <c r="B6" t="s">
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
+        <v>614</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1108</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>24703</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>20935</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1884.15</v>
       </c>
       <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>508</v>
-      </c>
-      <c r="K6" t="s">
-        <v>614</v>
-      </c>
-      <c r="L6" t="s">
-        <v>1108</v>
-      </c>
-      <c r="M6">
-        <v>24703</v>
-      </c>
-      <c r="N6">
-        <v>20935</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
         <v>1884.15</v>
       </c>
-      <c r="Q6">
-        <v>1884.15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>0</v>
+      <c r="B7" t="s">
+        <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
+        <v>683</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1109</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>46111</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>39077.5</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>3516.98</v>
       </c>
       <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>786</v>
-      </c>
-      <c r="K7" t="s">
-        <v>683</v>
-      </c>
-      <c r="L7" t="s">
-        <v>1109</v>
-      </c>
-      <c r="M7">
-        <v>46111</v>
-      </c>
-      <c r="N7">
-        <v>39077.5</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
         <v>3516.98</v>
       </c>
-      <c r="Q7">
-        <v>3516.98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" t="s">
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
+        <v>683</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1110</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>4863</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>4121.15</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>370.9</v>
       </c>
       <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>786</v>
-      </c>
-      <c r="K8" t="s">
-        <v>683</v>
-      </c>
-      <c r="L8" t="s">
-        <v>1110</v>
-      </c>
-      <c r="M8">
-        <v>4863</v>
-      </c>
-      <c r="N8">
-        <v>4121.15</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
         <v>370.9</v>
       </c>
-      <c r="Q8">
-        <v>370.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>0</v>
+      <c r="B9" t="s">
+        <v>151</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
+        <v>683</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1111</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>4880</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>4136</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>372.24</v>
       </c>
       <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>786</v>
-      </c>
-      <c r="K9" t="s">
-        <v>683</v>
-      </c>
-      <c r="L9" t="s">
-        <v>1111</v>
-      </c>
-      <c r="M9">
-        <v>4880</v>
-      </c>
-      <c r="N9">
-        <v>4136</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
         <v>372.24</v>
       </c>
-      <c r="Q9">
-        <v>372.24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>0</v>
+      <c r="B10" t="s">
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
+        <v>611</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1112</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>7797</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>6607</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>1496</v>
-      </c>
-      <c r="K10" t="s">
-        <v>611</v>
-      </c>
-      <c r="L10" t="s">
-        <v>1112</v>
-      </c>
-      <c r="M10">
-        <v>7797</v>
-      </c>
-      <c r="N10">
-        <v>6607</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
         <v>595</v>
       </c>
-      <c r="Q10">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>0</v>
+      <c r="B11" t="s">
+        <v>173</v>
       </c>
       <c r="C11" t="s">
-        <v>173</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
+        <v>682</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1113</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2825</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>2825</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>141.25</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -41945,211 +41153,115 @@
       <c r="I11">
         <v>0</v>
       </c>
-      <c r="J11">
-        <v>19001331</v>
-      </c>
-      <c r="K11" t="s">
-        <v>682</v>
-      </c>
-      <c r="L11" t="s">
-        <v>1113</v>
-      </c>
-      <c r="M11">
-        <v>2825</v>
-      </c>
-      <c r="N11">
-        <v>2825</v>
-      </c>
-      <c r="O11">
-        <v>141.25</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>0</v>
+      <c r="B12" t="s">
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
+        <v>643</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1114</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>743</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>630</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>56.7</v>
       </c>
       <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>71</v>
-      </c>
-      <c r="K12" t="s">
-        <v>643</v>
-      </c>
-      <c r="L12" t="s">
-        <v>1114</v>
-      </c>
-      <c r="M12">
-        <v>743</v>
-      </c>
-      <c r="N12">
-        <v>630</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
         <v>56.7</v>
       </c>
-      <c r="Q12">
-        <v>56.7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>0</v>
+      <c r="B13" t="s">
+        <v>113</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
+        <v>628</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1115</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>673</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>570</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>51.3</v>
       </c>
       <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>1012</v>
-      </c>
-      <c r="K13" t="s">
-        <v>628</v>
-      </c>
-      <c r="L13" t="s">
-        <v>1115</v>
-      </c>
-      <c r="M13">
-        <v>673</v>
-      </c>
-      <c r="N13">
-        <v>570</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
         <v>51.3</v>
       </c>
-      <c r="Q13">
-        <v>51.3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>0</v>
+      <c r="B14" t="s">
+        <v>99</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
+        <v>614</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1116</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>16072</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>13620</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1225.8</v>
       </c>
       <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>670</v>
-      </c>
-      <c r="K14" t="s">
-        <v>614</v>
-      </c>
-      <c r="L14" t="s">
-        <v>1116</v>
-      </c>
-      <c r="M14">
-        <v>16072</v>
-      </c>
-      <c r="N14">
-        <v>13620</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
         <v>1225.8</v>
       </c>
-      <c r="Q14">
-        <v>1225.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>0</v>
+      <c r="B15" t="s">
+        <v>173</v>
       </c>
       <c r="C15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
+        <v>682</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1117</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>2272</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>2272</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>113.6</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -42157,211 +41269,115 @@
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15">
-        <v>19002289</v>
-      </c>
-      <c r="K15" t="s">
-        <v>682</v>
-      </c>
-      <c r="L15" t="s">
-        <v>1117</v>
-      </c>
-      <c r="M15">
-        <v>2272</v>
-      </c>
-      <c r="N15">
-        <v>2272</v>
-      </c>
-      <c r="O15">
-        <v>113.6</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>0</v>
+      <c r="B16" t="s">
+        <v>108</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
+        <v>623</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1030</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>23503</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>19918</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>1792.62</v>
       </c>
       <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>115</v>
-      </c>
-      <c r="K16" t="s">
-        <v>623</v>
-      </c>
-      <c r="L16" t="s">
-        <v>1030</v>
-      </c>
-      <c r="M16">
-        <v>23503</v>
-      </c>
-      <c r="N16">
-        <v>19918</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
         <v>1792.62</v>
       </c>
-      <c r="Q16">
-        <v>1792.62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>0</v>
+      <c r="B17" t="s">
+        <v>157</v>
       </c>
       <c r="C17" t="s">
-        <v>157</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
+        <v>684</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1118</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>531</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>450</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>40.5</v>
       </c>
       <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>7</v>
-      </c>
-      <c r="K17" t="s">
-        <v>684</v>
-      </c>
-      <c r="L17" t="s">
-        <v>1118</v>
-      </c>
-      <c r="M17">
-        <v>531</v>
-      </c>
-      <c r="N17">
-        <v>450</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
         <v>40.5</v>
       </c>
-      <c r="Q17">
-        <v>40.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>0</v>
+      <c r="B18" t="s">
+        <v>102</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
+        <v>617</v>
+      </c>
+      <c r="D18" t="s">
+        <v>255</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>8922</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>7561</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>680.49</v>
       </c>
       <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>51</v>
-      </c>
-      <c r="K18" t="s">
-        <v>617</v>
-      </c>
-      <c r="L18" t="s">
-        <v>255</v>
-      </c>
-      <c r="M18">
-        <v>8922</v>
-      </c>
-      <c r="N18">
-        <v>7561</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
         <v>680.49</v>
       </c>
-      <c r="Q18">
-        <v>680.49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>0</v>
+      <c r="B19" t="s">
+        <v>173</v>
       </c>
       <c r="C19" t="s">
-        <v>173</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
+        <v>682</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1119</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>2030</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>2030</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>101.5</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -42369,187 +41385,91 @@
       <c r="I19">
         <v>0</v>
       </c>
-      <c r="J19">
-        <v>19002685</v>
-      </c>
-      <c r="K19" t="s">
-        <v>682</v>
-      </c>
-      <c r="L19" t="s">
-        <v>1119</v>
-      </c>
-      <c r="M19">
-        <v>2030</v>
-      </c>
-      <c r="N19">
-        <v>2030</v>
-      </c>
-      <c r="O19">
-        <v>101.5</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>0</v>
+      <c r="B20" t="s">
+        <v>174</v>
       </c>
       <c r="C20" t="s">
-        <v>174</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
+        <v>685</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1120</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1859</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1575</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>141.75</v>
       </c>
       <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>2212</v>
-      </c>
-      <c r="K20" t="s">
-        <v>685</v>
-      </c>
-      <c r="L20" t="s">
-        <v>1120</v>
-      </c>
-      <c r="M20">
-        <v>1859</v>
-      </c>
-      <c r="N20">
-        <v>1575</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
         <v>141.75</v>
       </c>
-      <c r="Q20">
-        <v>141.75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>0</v>
+      <c r="B21" t="s">
+        <v>136</v>
       </c>
       <c r="C21" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
+        <v>651</v>
+      </c>
+      <c r="D21" t="s">
+        <v>730</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>5735</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>4860.2</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>437.4</v>
       </c>
       <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>94</v>
-      </c>
-      <c r="K21" t="s">
-        <v>651</v>
-      </c>
-      <c r="L21" t="s">
-        <v>730</v>
-      </c>
-      <c r="M21">
-        <v>5735</v>
-      </c>
-      <c r="N21">
-        <v>4860.2</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
         <v>437.4</v>
       </c>
-      <c r="Q21">
-        <v>437.4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>0</v>
+      <c r="B22" t="s">
+        <v>135</v>
       </c>
       <c r="C22" t="s">
-        <v>135</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
+        <v>650</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1121</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>29500</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>2250</v>
       </c>
       <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>67</v>
-      </c>
-      <c r="K22" t="s">
-        <v>650</v>
-      </c>
-      <c r="L22" t="s">
-        <v>1121</v>
-      </c>
-      <c r="M22">
-        <v>29500</v>
-      </c>
-      <c r="N22">
-        <v>25000</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>2250</v>
-      </c>
-      <c r="Q22">
         <v>2250</v>
       </c>
     </row>

</xml_diff>